<commit_message>
Update Budgeting for expenses.xlsx
</commit_message>
<xml_diff>
--- a/Budgeting for expenses.xlsx
+++ b/Budgeting for expenses.xlsx
@@ -6401,8 +6401,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3F89B57BBFBFB488B76A7D1ADC9665A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="78f2bc3735b31513c37623e662c7329b">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e6b1fbe-b8f3-4d7a-becf-6ac8a51ab10f" xmlns:ns3="13abee14-ba4e-47f5-af47-cc96b3222db4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="540f19da467ce714c0da6fe0f771f56a" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F3F89B57BBFBFB488B76A7D1ADC9665A" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4621461c5f65802f11803ad16824a2f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2e6b1fbe-b8f3-4d7a-becf-6ac8a51ab10f" xmlns:ns3="13abee14-ba4e-47f5-af47-cc96b3222db4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="11e6a5ae1e78355c69a9b2a5b784bed9" ns2:_="" ns3:_="">
     <xsd:import namespace="2e6b1fbe-b8f3-4d7a-becf-6ac8a51ab10f"/>
     <xsd:import namespace="13abee14-ba4e-47f5-af47-cc96b3222db4"/>
     <xsd:element name="properties">
@@ -6621,7 +6621,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8E5F9F8-730C-4E01-BEF6-C3A52BCC7B8B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE0C8114-4170-48CE-A816-ECF8D6E358CE}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>